<commit_message>
replaced non ascii chars with ascii chars
</commit_message>
<xml_diff>
--- a/backend/app/records.xlsx
+++ b/backend/app/records.xlsx
@@ -1,115 +1,33 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11113"/>
-  <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nam/Documents/MA1/SEM 1/MMI/Recommender System/HCIPaper/backend/app/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EFBEBC30-8A36-AF42-BB9B-33248A2948A0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="760" yWindow="500" windowWidth="28040" windowHeight="16080" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="760" yWindow="500" windowWidth="28040" windowHeight="16080" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <definedNames/>
+  <calcPr calcId="0" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
-  <si>
-    <t>id</t>
-  </si>
-  <si>
-    <t>name1</t>
-  </si>
-  <si>
-    <t>image1</t>
-  </si>
-  <si>
-    <t>description1</t>
-  </si>
-  <si>
-    <t>summary1</t>
-  </si>
-  <si>
-    <t>name2</t>
-  </si>
-  <si>
-    <t>image2</t>
-  </si>
-  <si>
-    <t>description2</t>
-  </si>
-  <si>
-    <t>summary2</t>
-  </si>
-  <si>
-    <t>name3</t>
-  </si>
-  <si>
-    <t>image3</t>
-  </si>
-  <si>
-    <t>description3</t>
-  </si>
-  <si>
-    <t>summary3</t>
-  </si>
-  <si>
-    <t>name4</t>
-  </si>
-  <si>
-    <t>image4</t>
-  </si>
-  <si>
-    <t>description4</t>
-  </si>
-  <si>
-    <t>summary4</t>
-  </si>
-  <si>
-    <t>startTime</t>
-  </si>
-  <si>
-    <t>endTime</t>
-  </si>
-  <si>
-    <t>formType</t>
-  </si>
-  <si>
-    <t>V1</t>
-  </si>
-  <si>
-    <t>V2</t>
-  </si>
-  <si>
-    <t>V3</t>
-  </si>
-  <si>
-    <t>finalTime</t>
-  </si>
-</sst>
-</file>
-
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="0"/>
+  <fonts count="1">
     <font>
-      <sz val="12"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <color theme="1"/>
+      <sz val="12"/>
       <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill patternType="none"/>
+      <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -128,21 +46,80 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
@@ -442,90 +419,452 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:X1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:AB3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
-    <col min="1" max="1" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col width="12.1640625" bestFit="1" customWidth="1" min="1" max="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" t="s">
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>id</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>name1</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>image1</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>description1</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>summary1</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>name2</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>image2</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>description2</t>
+        </is>
+      </c>
+      <c r="I1" t="inlineStr">
+        <is>
+          <t>summary2</t>
+        </is>
+      </c>
+      <c r="J1" t="inlineStr">
+        <is>
+          <t>name3</t>
+        </is>
+      </c>
+      <c r="K1" t="inlineStr">
+        <is>
+          <t>image3</t>
+        </is>
+      </c>
+      <c r="L1" t="inlineStr">
+        <is>
+          <t>description3</t>
+        </is>
+      </c>
+      <c r="M1" t="inlineStr">
+        <is>
+          <t>summary3</t>
+        </is>
+      </c>
+      <c r="N1" t="inlineStr">
+        <is>
+          <t>name4</t>
+        </is>
+      </c>
+      <c r="O1" t="inlineStr">
+        <is>
+          <t>image4</t>
+        </is>
+      </c>
+      <c r="P1" t="inlineStr">
+        <is>
+          <t>description4</t>
+        </is>
+      </c>
+      <c r="Q1" t="inlineStr">
+        <is>
+          <t>summary4</t>
+        </is>
+      </c>
+      <c r="R1" t="inlineStr">
+        <is>
+          <t>startTime</t>
+        </is>
+      </c>
+      <c r="S1" t="inlineStr">
+        <is>
+          <t>endTime</t>
+        </is>
+      </c>
+      <c r="T1" t="inlineStr">
+        <is>
+          <t>formType</t>
+        </is>
+      </c>
+      <c r="U1" t="inlineStr">
+        <is>
+          <t>V1</t>
+        </is>
+      </c>
+      <c r="V1" t="inlineStr">
+        <is>
+          <t>V2</t>
+        </is>
+      </c>
+      <c r="W1" t="inlineStr">
+        <is>
+          <t>V3</t>
+        </is>
+      </c>
+      <c r="X1" t="inlineStr">
+        <is>
+          <t>finalTime</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="n">
+        <v>4751920640</v>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>Zuma</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>https://dierenasielgenk.be/wp-content/uploads/2021/08/zumaa.jpg</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>Zuma heeft nogal een weg afgelegd vóór hij in ons asiel terecht is gekomen. Van de fokker is hij naar de eerste eigenaar gegaan, waar hij moeite had met het kind van de eigenaar. Hierop is hij doorgegeven aan mensen die zich niet bewust zijn van wat houden van honden inhoudt, zowel letterlijk als figuurlijk. Zuma is vervolgens op straat gezet en gelukkig veilig gevangen door onze hondenvanger.
+U kunt dus wel stellen dat Zuma een slechte start heeft gehad.
+In nieuwe situaties is hij erg onderzoekend en wil daarbij alles besnuffelen. Rondom nieuwe personen is hij onzeker en hij vertrouwt ook niet iedereen gelijk. Er is een vermoeden dat Zuma fysiek niet altijd even goed behandeld is geweest. We vinden het daarom belangrijk om aan zijn nieuwe eigenaren uitleg te geven over signalen die hij geeft wanneer hij zich minder comfortabel voelt. Het is nog geen hond die geniet van lange knuffelsessies.
+Waar je Zuma wel blij mee kunt maken is speuren. Hij is voergevoelig en hij kent ook al verschillende commando’s, zoals zit, af, poot en blijf. Speeltjes zijn fantastisch en er is veel met Zuma gewerkt met trekspellen. We zien dat Zuma hierin etiquette nodig gaat hebben, zodat spel gecontroleerd blijft.
+Wandelen is wel gekend door Zuma, maar het is nog geen hele ontspannen bezigheid. Hier kan de nieuwe eigenaar zeker aan werken!
+Wij weten zeker dat Zuma een mooie band kan gaan opbouwen met zijn nieuwe eigenaar wanneer hij deze gaat vertrouwen en er samen leuke en fijne dingen worden gedaan met hem.  
+Voor Zuma zoeken we een huis met een tuin, zonder kinderen. Hij kan eventueel bij een leuk teefje worden geplaatst.
+Bij interesse stuurt u het best een mailtje naar info@dierenasielgenk.be
+Deze hond zit in het programma van Belgian Cell Dogs, waarbij gedetineerden trainen met asielhonden om zodoende de adoptiekansen van de honden te verhogen. De honden leren commando’s en gewenst gedrag te vertonen.
+Gedurende 8 weken wordt de hond getraind en in die tijd kunnen adoptanten zich heel graag aanmelden voor de hond, kunnen er adoptie gesprekken plaatsvinden én kunnen adoptanten kijken hoe er vanuit Belgian Cell Dogs wordt getraind. De adoptie vindt dan plaats na het programma van 8 weken.</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>Ik ben op zoek naar een baasje om mee te spelen en te speuren en om samen een mooie band op te bouwen!</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>https://dierenasielgenk.be/honden/zuma/</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>Rita</t>
+        </is>
+      </c>
+      <c r="H2" t="inlineStr">
+        <is>
+          <t>https://dierenasielgenk.be/wp-content/uploads/2021/07/rita-1200x1800.jpg</t>
+        </is>
+      </c>
+      <c r="I2" t="inlineStr">
+        <is>
+          <t>Rita is een Duitse Herder van 2014. Ze werd gevonden, maar bleek afkomstig van mensen die bekend zijn omwille van het niet goed verzorgen van dieren.
+Helaas hebben we geen informatie over het verleden van Rita.
+Bij binnenkomst had Rita een oorontsteking aan beide oren. Ze heeft hiervoor een behandeling gekregen en heeft daar nu geen last meer van.
+Rita heeft even tijd nodig om mensen te leren kennen. Ze is geen allemansvriend, maar ze laat zich gelukkig goed omkopen met lekkere snoepjes. Dit is haar grote pluspunt, ook bij het leren van nieuwe commando’s en tijdens wandelingen. Hierdoor is ze goed af te leiden bij het zien van prikkels.
+Ze heeft duidelijk in huis geleefd en voelt zich comfortabel binnenshuis.
+Rita speelt ook graag. Tennisballen vindt ze heel fijn, net als pluche knuffels. We zien ook dat ze meer en meer vraagt om geknuffeld te worden door mensen die ze kent.
+Deze lieve, zachte dame is op zoek naar een rustige thuis met een tuin. Ze houdt niet zo van andere dieren en kinderen.
+Deze hond zit in het programma van Belgian Cell Dogs, waarbij gedetineerden trainen met asielhonden om zodoende de adoptiekansen van de honden te verhogen. De honden leren commando’s en gewenst gedrag te vertonen.
+Gedurende 8 weken wordt de hond getraind en in die tijd kunnen adoptanten zich heel graag aanmelden voor de hond, kunnen er adoptie gesprekken plaatsvinden én kunnen adoptanten kijken hoe er vanuit Belgian Cell Dogs wordt getraind. De adoptie vindt dan plaats na het programma van 8 weken.</t>
+        </is>
+      </c>
+      <c r="J2" t="inlineStr">
+        <is>
+          <t>Ik ben geen allemansvriend, maar ik ben gek op snoepjes, spelen en knuffelen met bekende mensen!</t>
+        </is>
+      </c>
+      <c r="K2" t="inlineStr">
+        <is>
+          <t>https://dierenasielgenk.be/honden/rita/</t>
+        </is>
+      </c>
+      <c r="L2" t="inlineStr">
+        <is>
+          <t>Molly</t>
+        </is>
+      </c>
+      <c r="M2" t="inlineStr">
+        <is>
+          <t>https://dierenasielgenk.be/wp-content/uploads/2020/05/IMG_7834-3-1200x801.jpg</t>
+        </is>
+      </c>
+      <c r="N2" t="inlineStr">
+        <is>
+          <t>Er zijn zo van die honden die bijna horen tot het ‘vaste meubilair’ van het asiel. Zonde, want we begrijpen vaak zelf niet goed hoe dat komt.
+Een van die honden is Mechelaar Molly.
+Deze pittige dame wordt geschat op zo’n zes jaar oud. Haar leven liep tot hiertoe allesbehalve over rozen. Ze werd gehouden als kweekteefje, maar na bewezen diensten ‘bedankt’ door haar te dumpen langs de kant van de weg.
+Toch laat Molly haar mooie kopje daar niet door hangen, want ze ontpopte zich in het asiel tot een energieke, leergierige hond. Haar grote passie? Heerlijk achter de bal stuiteren. Ze houdt je liefst uren bezig met balletje gooien. Maar een andere activiteit waar deze atlete gek op is, is zwemmen. Zoek je zwemmaatje? Dan is Molly zeker en vast van de partij!
+Een kus van de juf en een bank vooruit
+Tijdens haar lange verblijf in het asiel, werd er al grondig getraind met Molly. Want in het begin reageerde ze tijdens een wandeling op alles wat bewoog, maar inmiddels gedraagt ze zich al erg flink! We merkten ook heel duidelijk dat ze enorm leergierig is. Er is dus nog veel ruimte om te groeien.
+Molly kan niet geplaatst worden bij andere dieren of kleine kinderen en een hoge omheining is een must voor deze schone springster. 
+Zoek je dus een trouwe metgezel om stap voor stap te laten kennismaken met het huiselijke leven? Dan is Molly misschien wel je ideale match!</t>
+        </is>
+      </c>
+      <c r="O2" t="inlineStr">
+        <is>
+          <t>Zoek je een trouwe, leergierige metgezel om verder te laten kennismaken met het huiselijke leven? Dan is Molly misschien wel je ideale match!</t>
+        </is>
+      </c>
+      <c r="P2" t="inlineStr">
+        <is>
+          <t>https://dierenasielgenk.be/honden/molly/</t>
+        </is>
+      </c>
+      <c r="Q2" t="inlineStr">
+        <is>
+          <t>Thor</t>
+        </is>
+      </c>
+      <c r="R2" t="inlineStr">
+        <is>
+          <t>https://dierenasielgenk.be/wp-content/uploads/2022/08/IMG_8797.1jpg-1200x800.jpg</t>
+        </is>
+      </c>
+      <c r="S2" t="inlineStr">
+        <is>
+          <t>Thor werd uit een donkere stal gehaald, helemaal achterin de tuin. Het was al even geleden dat Thor uit de stal was geweest: er werd niet gewandeld met Thor en ook in huis komen was geen optie. Sterker nog: op het moment dat Thor in beslag werd genomen, gaf de eigenaar al aan ‘Thor niet meer te willen’. Thor was in de ogen van zijn vorige eigenaar niet meer dan een object, waar hij in het asiel eindelijk weer ‘hond’ mocht zijn. Hij mocht zijn pootjes strekken, rondlopen in de speelweide en hij kreeg weer eens fysiek contact.
+Deze man is geboren in mei 2015 en zou graag de rest van zijn leven willen doorbrengen op een plaats waar hij wel graag gezien wordt, waar hij voldoende eten krijgt en waar hij goed verzorgd wordt.
+In het asiel heeft Thor onmiddellijk laten zien wat hij goed kan: hoog springen. Hij vond het zo fijn om zijn poten eens te kunnen strekken, dat hij dit iets té enthousiast heeft gedaan. Belangrijk punt voor zijn nieuwe eigenaren is dus een voldoende hoge omheining.
+Door al die jaren in duisternis te leven, waren heel veel dingen eng voor Thor. Hij heeft in het asiel veel geleerd: knuffels krijgen is heel leuk, wandelen is heel fijn en mensen dienen niet om je ergens in op te sluiten, maar om samen iets met je te doen!
+Waar Thor in het begin heel veel moeite had met alle prikkels in het asiel, zien we nu vreugde wanneer hij bekenden ziet. Hij begint te piepen en schudt met zijn hele achterwerk van enthousiasme!
+Een zindelijkheidstraining is voor Thor gewenst, evenals een huis met een tuin.
+Deze vriendelijke man moet nog veel leren, maar hij wil ontzettend graag! Bij rustige, geduldige mensen die in het begin meer thuis zijn, zal hij veel stappen kunnen zetten. Liefst ook letterlijk, want het leven opnieuw doorbrengen in een stal, is geen optie meer. Thor zou herplaatst kunnen worden bij een een stabiele en steriele teef.</t>
+        </is>
+      </c>
+      <c r="T2" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Ik zou heel graag de rest van mijn leven doorbrengen op een plek waar ik graag gezien wordt, voldoende eten krijg en goed verzorgd wordt. </t>
+        </is>
+      </c>
+      <c r="U2" t="inlineStr">
+        <is>
+          <t>https://dierenasielgenk.be/honden/thor/</t>
+        </is>
+      </c>
+      <c r="V2" t="inlineStr">
+        <is>
+          <t>11:35:45</t>
+        </is>
+      </c>
+      <c r="W2" t="inlineStr">
+        <is>
+          <t>11:35:51</t>
+        </is>
+      </c>
+      <c r="X2" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="n">
+        <v>4750523968</v>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>Zuma</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>https://dierenasielgenk.be/wp-content/uploads/2021/08/zumaa.jpg</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>Zuma heeft nogal een weg afgelegd vóór hij in ons asiel terecht is gekomen. Van de fokker is hij naar de eerste eigenaar gegaan, waar hij moeite had met het kind van de eigenaar. Hierop is hij doorgegeven aan mensen die zich niet bewust zijn van wat houden van honden inhoudt, zowel letterlijk als figuurlijk. Zuma is vervolgens op straat gezet en gelukkig veilig gevangen door onze hondenvanger.
+U kunt dus wel stellen dat Zuma een slechte start heeft gehad.
+In nieuwe situaties is hij erg onderzoekend en wil daarbij alles besnuffelen. Rondom nieuwe personen is hij onzeker en hij vertrouwt ook niet iedereen gelijk. Er is een vermoeden dat Zuma fysiek niet altijd even goed behandeld is geweest. We vinden het daarom belangrijk om aan zijn nieuwe eigenaren uitleg te geven over signalen die hij geeft wanneer hij zich minder comfortabel voelt. Het is nog geen hond die geniet van lange knuffelsessies.
+Waar je Zuma wel blij mee kunt maken is speuren. Hij is voergevoelig en hij kent ook al verschillende commando’s, zoals zit, af, poot en blijf. Speeltjes zijn fantastisch en er is veel met Zuma gewerkt met trekspellen. We zien dat Zuma hierin etiquette nodig gaat hebben, zodat spel gecontroleerd blijft.
+Wandelen is wel gekend door Zuma, maar het is nog geen hele ontspannen bezigheid. Hier kan de nieuwe eigenaar zeker aan werken!
+Wij weten zeker dat Zuma een mooie band kan gaan opbouwen met zijn nieuwe eigenaar wanneer hij deze gaat vertrouwen en er samen leuke en fijne dingen worden gedaan met hem.  
+Voor Zuma zoeken we een huis met een tuin, zonder kinderen. Hij kan eventueel bij een leuk teefje worden geplaatst.
+Bij interesse stuurt u het best een mailtje naar info@dierenasielgenk.be
+Deze hond zit in het programma van Belgian Cell Dogs, waarbij gedetineerden trainen met asielhonden om zodoende de adoptiekansen van de honden te verhogen. De honden leren commando’s en gewenst gedrag te vertonen.
+Gedurende 8 weken wordt de hond getraind en in die tijd kunnen adoptanten zich heel graag aanmelden voor de hond, kunnen er adoptie gesprekken plaatsvinden én kunnen adoptanten kijken hoe er vanuit Belgian Cell Dogs wordt getraind. De adoptie vindt dan plaats na het programma van 8 weken.</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>Ik ben op zoek naar een baasje om mee te spelen en te speuren en om samen een mooie band op te bouwen!</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>https://dierenasielgenk.be/honden/zuma/</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>Thor</t>
+        </is>
+      </c>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>https://dierenasielgenk.be/wp-content/uploads/2022/08/IMG_8797.1jpg-1200x800.jpg</t>
+        </is>
+      </c>
+      <c r="I3" t="inlineStr">
+        <is>
+          <t>Thor werd uit een donkere stal gehaald, helemaal achterin de tuin. Het was al even geleden dat Thor uit de stal was geweest: er werd niet gewandeld met Thor en ook in huis komen was geen optie. Sterker nog: op het moment dat Thor in beslag werd genomen, gaf de eigenaar al aan ‘Thor niet meer te willen’. Thor was in de ogen van zijn vorige eigenaar niet meer dan een object, waar hij in het asiel eindelijk weer ‘hond’ mocht zijn. Hij mocht zijn pootjes strekken, rondlopen in de speelweide en hij kreeg weer eens fysiek contact.
+Deze man is geboren in mei 2015 en zou graag de rest van zijn leven willen doorbrengen op een plaats waar hij wel graag gezien wordt, waar hij voldoende eten krijgt en waar hij goed verzorgd wordt.
+In het asiel heeft Thor onmiddellijk laten zien wat hij goed kan: hoog springen. Hij vond het zo fijn om zijn poten eens te kunnen strekken, dat hij dit iets té enthousiast heeft gedaan. Belangrijk punt voor zijn nieuwe eigenaren is dus een voldoende hoge omheining.
+Door al die jaren in duisternis te leven, waren heel veel dingen eng voor Thor. Hij heeft in het asiel veel geleerd: knuffels krijgen is heel leuk, wandelen is heel fijn en mensen dienen niet om je ergens in op te sluiten, maar om samen iets met je te doen!
+Waar Thor in het begin heel veel moeite had met alle prikkels in het asiel, zien we nu vreugde wanneer hij bekenden ziet. Hij begint te piepen en schudt met zijn hele achterwerk van enthousiasme!
+Een zindelijkheidstraining is voor Thor gewenst, evenals een huis met een tuin.
+Deze vriendelijke man moet nog veel leren, maar hij wil ontzettend graag! Bij rustige, geduldige mensen die in het begin meer thuis zijn, zal hij veel stappen kunnen zetten. Liefst ook letterlijk, want het leven opnieuw doorbrengen in een stal, is geen optie meer. Thor zou herplaatst kunnen worden bij een een stabiele en steriele teef.</t>
+        </is>
+      </c>
+      <c r="J3" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Ik zou heel graag de rest van mijn leven doorbrengen op een plek waar ik graag gezien wordt, voldoende eten krijg en goed verzorgd wordt. </t>
+        </is>
+      </c>
+      <c r="K3" t="inlineStr">
+        <is>
+          <t>https://dierenasielgenk.be/honden/thor/</t>
+        </is>
+      </c>
+      <c r="L3" t="inlineStr">
+        <is>
+          <t>Henkie</t>
+        </is>
+      </c>
+      <c r="M3" t="inlineStr">
+        <is>
+          <t>https://dierenasielgenk.be/wp-content/uploads/2022/10/20221007_175756-1200x1814.jpg</t>
+        </is>
+      </c>
+      <c r="N3" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Deze leuke en lieve Lhasa Apso is na een hobbelig verleden op zoek naar een liefdevol thuis.
+Henkie is door een inbeslagname bij ons binnengebracht samen met nog enkele andere hondjes. Ze werden gebruikt voor de fok, maar kregen niet de juiste verzorging. Henkies vacht was vervilt, hij had kale plekken op zijn lijf en zijn ogen waren er slecht aan toe.
+Toch kwam gelijk zijn vrolijke en vriendelijke karakter naar boven ondanks dat hij in een nieuwe omgeving terecht kwam en zijn zicht vrijwel volledig ontbrak. Hij onderzocht zijn nieuwe plekje en was blij met de aandacht die hij kreeg. Hij is ook erg speels en vindt alle speeltjes leuk
+Op dit moment zit Henkie in een gastgezin waar hij veel liefde krijgt, hondenvriendjes heeft en ook de nodige medische zorg ontvangt. Ondertussen is hij gecastreerd, is zijn rechteroogje weggenomen en is zijn huid en vacht onder handen genomen. Om zijn andere oog te behouden wordt hij dagelijks intensief gezalfd en in de nabije toekomst heeft hij nog een operatie aan zijn knie nodig. We zoeken baasjes die deze zorg verder willen opvolgen.
+Henkie is 6 jaar, hij is zachtaardig, vriendelijk, onderzoekend en een levensgenieter. Hij wordt uitsluitend geplaatst bij een andere hond, hij kan ook bij kinderen vanaf 10 jaar en hij heeft nood aan een omheinde tuin. 
+In een nieuw thuis heeft Henkie veel baat bij een ander hondje en zullen aspecten zoals zindelijkheid en wandelen aan de riem verder opgebouwd moeten worden. In het gastgezin heeft hij hier al veel stappen in gemaakt.
+</t>
+        </is>
+      </c>
+      <c r="O3" t="inlineStr">
+        <is>
+          <t>Ik heb nog wat extra zorg en aandacht nodig, maar ik ben vrolijk, vriendelijk, speels en ik houd van aandacht!</t>
+        </is>
+      </c>
+      <c r="P3" t="inlineStr">
+        <is>
+          <t>https://dierenasielgenk.be/honden/henkie-3/</t>
+        </is>
+      </c>
+      <c r="Q3" t="inlineStr">
+        <is>
+          <t>Lucky</t>
+        </is>
+      </c>
+      <c r="R3" t="inlineStr">
+        <is>
+          <t>https://dierenasielgenk.be/wp-content/uploads/2022/11/IMG20221104163040-1200x900.jpg</t>
+        </is>
+      </c>
+      <c r="S3" t="inlineStr">
+        <is>
+          <t>Overgekomen vanuit Roemenië is Lucky nu als inbeslagname in ons asiel beland.
+We hopen dat snel het tij van onge-Lucky gaat keren en dat hij in een nieuw thuis veel geluk mag gaan ervaren.
+We hebben Lucky leren kennen als een onzekere hond die wel erg nieuwsgierig is en op onderzoek uit gaat. In eerste instantie zijn nieuwe dingen eng, maar met de juiste begeleiding is hij wel te sturen en durft hij dingen te onderzoeken.
+Hij is graag bij mensen die hij vertrouwt en is dan een knuffelaar. Daarnaast speelt hij graag met mensen en met speeltjes en eet hij graag vleesjes. Aan wat commando’s zal nog gewerkt moeten worden.
+De deuren in zijn nieuwe thuis kunnen het best Lucky-proof zijn doordat hij deze graag open maakt om van de buitenlucht te genieten. Hij is graag buiten en snuffelt er dan op los.
+We zoeken voor Lucky een huis met een tuin waar gewerkt kan worden aan het vertrouwen tussen hem en zijn nieuwe baasje(s) en welke begrijpen dat Lucky niet in alle situaties de meest open en sociale hond is. Oudere kinderen en eventueel een stabiel teefje behoren tot de mogelijkheden.</t>
+        </is>
+      </c>
+      <c r="T3" t="inlineStr">
+        <is>
+          <t>Ik ben onzeker maar wel erg nieuwsgierig en als ik je vertrouw ben ik een echte knuffelaar en speelvogel!</t>
+        </is>
+      </c>
+      <c r="U3" t="inlineStr">
+        <is>
+          <t>https://dierenasielgenk.be/honden/lucky-2/</t>
+        </is>
+      </c>
+      <c r="V3" t="inlineStr">
+        <is>
+          <t>11:36:31</t>
+        </is>
+      </c>
+      <c r="W3" t="inlineStr">
+        <is>
+          <t>11:36:45</t>
+        </is>
+      </c>
+      <c r="X3" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="Y3" t="n">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" t="s">
-        <v>7</v>
-      </c>
-      <c r="I1" t="s">
-        <v>8</v>
-      </c>
-      <c r="J1" t="s">
-        <v>9</v>
-      </c>
-      <c r="K1" t="s">
-        <v>10</v>
-      </c>
-      <c r="L1" t="s">
-        <v>11</v>
-      </c>
-      <c r="M1" t="s">
-        <v>12</v>
-      </c>
-      <c r="N1" t="s">
-        <v>13</v>
-      </c>
-      <c r="O1" t="s">
-        <v>14</v>
-      </c>
-      <c r="P1" t="s">
-        <v>15</v>
-      </c>
-      <c r="Q1" t="s">
-        <v>16</v>
-      </c>
-      <c r="R1" t="s">
-        <v>17</v>
-      </c>
-      <c r="S1" t="s">
-        <v>18</v>
-      </c>
-      <c r="T1" t="s">
-        <v>19</v>
-      </c>
-      <c r="U1" t="s">
-        <v>20</v>
-      </c>
-      <c r="V1" t="s">
-        <v>21</v>
-      </c>
-      <c r="W1" t="s">
-        <v>22</v>
-      </c>
-      <c r="X1" t="s">
-        <v>23</v>
+      <c r="Z3" t="n">
+        <v>4</v>
+      </c>
+      <c r="AA3" t="n">
+        <v>4</v>
+      </c>
+      <c r="AB3" t="inlineStr">
+        <is>
+          <t>11:38:29</t>
+        </is>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
BUG FIX MAKE RECOMMENDATION: reset all scores per fetch request + updated dataset
</commit_message>
<xml_diff>
--- a/backend/app/records.xlsx
+++ b/backend/app/records.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nam/Documents/MA1/SEM 1/MMI/Recommender System/HCIPaper/backend/app/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EFBEBC30-8A36-AF42-BB9B-33248A2948A0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{662D6F20-3C96-3B44-B5A5-42AC2444D71F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="760" yWindow="500" windowWidth="28040" windowHeight="16080" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -446,7 +446,7 @@
   <dimension ref="A1:X1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D21" sqref="D21"/>
+      <selection activeCell="AC30" sqref="A20:AC30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>